<commit_message>
Se realizo el primer caso de prueba
</commit_message>
<xml_diff>
--- a/src/main/resources/Data/data.xlsx
+++ b/src/main/resources/Data/data.xlsx
@@ -12,11 +12,12 @@
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>TituloCP</t>
   </si>
@@ -72,9 +73,6 @@
     <t>Dato17</t>
   </si>
   <si>
-    <t>Registro_OK</t>
-  </si>
-  <si>
     <t>Registro_NOK</t>
   </si>
   <si>
@@ -94,6 +92,12 @@
   </si>
   <si>
     <t>ividambo@gmail.com</t>
+  </si>
+  <si>
+    <t>CP00_registro_ok</t>
+  </si>
+  <si>
+    <t>Your registration completed</t>
   </si>
 </sst>
 </file>
@@ -140,9 +144,10 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -441,7 +446,7 @@
   <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -509,36 +514,39 @@
     </row>
     <row r="2" spans="1:18">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
         <v>22</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>23</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="F2">
         <v>123456</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:18">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
         <v>22</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>23</v>
-      </c>
-      <c r="D3" t="s">
-        <v>24</v>
       </c>
       <c r="F3">
         <v>123456</v>
@@ -546,12 +554,12 @@
     </row>
     <row r="4" spans="1:18">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:18">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -559,6 +567,7 @@
     <hyperlink ref="E2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Agregamos LoginOK and RegisterNO_OK
</commit_message>
<xml_diff>
--- a/src/main/resources/Data/data.xlsx
+++ b/src/main/resources/Data/data.xlsx
@@ -8,16 +8,13 @@
   </bookViews>
   <sheets>
     <sheet name="DataPrueba" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
-    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>TituloCP</t>
   </si>
@@ -37,51 +34,6 @@
     <t>Dato5</t>
   </si>
   <si>
-    <t>Dato6</t>
-  </si>
-  <si>
-    <t>Dato7</t>
-  </si>
-  <si>
-    <t>Dato8</t>
-  </si>
-  <si>
-    <t>Dato9</t>
-  </si>
-  <si>
-    <t>Dato10</t>
-  </si>
-  <si>
-    <t>Dato11</t>
-  </si>
-  <si>
-    <t>Dato12</t>
-  </si>
-  <si>
-    <t>Dato13</t>
-  </si>
-  <si>
-    <t>Dato14</t>
-  </si>
-  <si>
-    <t>Dato15</t>
-  </si>
-  <si>
-    <t>Dato16</t>
-  </si>
-  <si>
-    <t>Dato17</t>
-  </si>
-  <si>
-    <t>Registro_NOK</t>
-  </si>
-  <si>
-    <t>Login_OK</t>
-  </si>
-  <si>
-    <t>Compra_Articulo</t>
-  </si>
-  <si>
     <t>male</t>
   </si>
   <si>
@@ -91,20 +43,53 @@
     <t>dambo</t>
   </si>
   <si>
-    <t>ividambo@gmail.com</t>
-  </si>
-  <si>
-    <t>CP00_registro_ok</t>
-  </si>
-  <si>
     <t>Your registration completed</t>
+  </si>
+  <si>
+    <t>prueba_1@gmail.com</t>
+  </si>
+  <si>
+    <t>CP05 Agregar item carrito</t>
+  </si>
+  <si>
+    <t>CP004 LOGOUT</t>
+  </si>
+  <si>
+    <t>CP07 SubNewsletter</t>
+  </si>
+  <si>
+    <t>cuentanoexiste@gmail.com</t>
+  </si>
+  <si>
+    <t>manu</t>
+  </si>
+  <si>
+    <t>san</t>
+  </si>
+  <si>
+    <t>CP01RegistroNOOK</t>
+  </si>
+  <si>
+    <t>CP00registrook</t>
+  </si>
+  <si>
+    <t>The password should have at least 6 characters.</t>
+  </si>
+  <si>
+    <t>CP02Login_OK</t>
+  </si>
+  <si>
+    <t>CP03 LoginUserInvalido</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LoginPassInvalido </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -119,21 +104,50 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -144,10 +158,19 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -443,154 +466,169 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R5"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.42578125" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="42.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="E2" s="2">
+        <v>123456</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="2">
+        <v>12</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="C4" s="2">
+        <v>123456</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="2">
+        <v>123456</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="2">
+        <v>123</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18">
-      <c r="A2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2">
-        <v>123456</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18">
-      <c r="A3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3">
-        <v>123456</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18">
-      <c r="A4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18">
-      <c r="A5" t="s">
-        <v>20</v>
-      </c>
+      <c r="B9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="D10" s="1"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="C15" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="B4" r:id="rId1"/>
+    <hyperlink ref="B5" r:id="rId2"/>
+    <hyperlink ref="B8" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Agrego CP03 y CP07
</commit_message>
<xml_diff>
--- a/src/main/resources/Data/data.xlsx
+++ b/src/main/resources/Data/data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>TituloCP</t>
   </si>
@@ -55,9 +55,6 @@
     <t>CP004 LOGOUT</t>
   </si>
   <si>
-    <t>CP07 SubNewsletter</t>
-  </si>
-  <si>
     <t>cuentanoexiste@gmail.com</t>
   </si>
   <si>
@@ -79,10 +76,19 @@
     <t>CP02Login_OK</t>
   </si>
   <si>
-    <t>CP03 LoginUserInvalido</t>
-  </si>
-  <si>
     <t xml:space="preserve">LoginPassInvalido </t>
+  </si>
+  <si>
+    <t>CP03LoginUserInvalido</t>
+  </si>
+  <si>
+    <t>Login was unsuccessful. Please correct the errors and try again.</t>
+  </si>
+  <si>
+    <t>CP07SubNewsletter</t>
+  </si>
+  <si>
+    <t>Thank you for signing up! A verification email has been sent. We appreciate your interest.</t>
   </si>
 </sst>
 </file>
@@ -113,7 +119,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -123,6 +129,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -158,7 +176,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -167,10 +185,20 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -469,7 +497,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -477,98 +505,100 @@
     <col min="1" max="1" width="24.42578125" customWidth="1"/>
     <col min="2" max="2" width="28.7109375" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="81.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.42578125" customWidth="1"/>
     <col min="6" max="6" width="42.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="4">
+        <v>123456</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="4">
+        <v>12</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="2">
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="4">
         <v>123456</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="2">
-        <v>12</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="2">
+      <c r="D4" s="7"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="4">
         <v>123456</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="2">
-        <v>123456</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+      <c r="D5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="2" t="s">
@@ -592,7 +622,7 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>10</v>
@@ -605,16 +635,20 @@
       <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="2" t="s">
+      <c r="A9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+      <c r="C9" s="4">
+        <v>123456</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:6">
       <c r="D10" s="1"/>
@@ -627,8 +661,9 @@
     <hyperlink ref="B4" r:id="rId1"/>
     <hyperlink ref="B5" r:id="rId2"/>
     <hyperlink ref="B8" r:id="rId3"/>
+    <hyperlink ref="B9" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se finalizo caso 6 y caso 4
</commit_message>
<xml_diff>
--- a/src/main/resources/Data/data.xlsx
+++ b/src/main/resources/Data/data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t>TituloCP</t>
   </si>
@@ -49,9 +49,6 @@
     <t>prueba_1@gmail.com</t>
   </si>
   <si>
-    <t>CP004 LOGOUT</t>
-  </si>
-  <si>
     <t>cuentanoexiste@gmail.com</t>
   </si>
   <si>
@@ -73,9 +70,6 @@
     <t>CP02Login_OK</t>
   </si>
   <si>
-    <t xml:space="preserve">LoginPassInvalido </t>
-  </si>
-  <si>
     <t>CP03LoginUserInvalido</t>
   </si>
   <si>
@@ -92,6 +86,21 @@
   </si>
   <si>
     <t>Build your own cheap computer</t>
+  </si>
+  <si>
+    <t>CP06LoginPassInvalido</t>
+  </si>
+  <si>
+    <t>The credentials provided are incorrect</t>
+  </si>
+  <si>
+    <t>Excellent</t>
+  </si>
+  <si>
+    <t>CP004VoteCommunityPollSinLoggear</t>
+  </si>
+  <si>
+    <t>Only registered users can vote.</t>
   </si>
 </sst>
 </file>
@@ -122,18 +131,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -179,10 +182,13 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -191,18 +197,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -501,164 +501,170 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A2" sqref="A2:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" customWidth="1"/>
+    <col min="1" max="1" width="44.42578125" customWidth="1"/>
     <col min="2" max="2" width="28.7109375" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="32.28515625" customWidth="1"/>
     <col min="4" max="4" width="81.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.42578125" customWidth="1"/>
     <col min="6" max="6" width="42.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2">
+        <v>123456</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="2">
+        <v>12</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="4">
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2">
         <v>123456</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="4">
-        <v>12</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="4" t="s">
+      <c r="D4" s="9"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="4">
+      <c r="B5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="2">
         <v>123456</v>
       </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="4">
-        <v>123456</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
+      <c r="D5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
+      <c r="A6" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>28</v>
+      </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="6" t="s">
+      <c r="A7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="2">
         <v>123456</v>
       </c>
-      <c r="D7" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
+      <c r="D7" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="2">
         <v>123</v>
       </c>
-      <c r="D8" s="2"/>
+      <c r="D8" s="8" t="s">
+        <v>25</v>
+      </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="6" t="s">
+      <c r="A9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="2">
         <v>123456</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
+      <c r="D9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
     </row>
     <row r="10" spans="1:6">
       <c r="D10" s="1"/>

</xml_diff>

<commit_message>
agregando test a testng.xml
</commit_message>
<xml_diff>
--- a/src/main/resources/Data/data.xlsx
+++ b/src/main/resources/Data/data.xlsx
@@ -501,7 +501,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -605,7 +605,7 @@
       <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>26</v>
       </c>
       <c r="B6" s="7" t="s">

</xml_diff>